<commit_message>
added test cases & documentation
</commit_message>
<xml_diff>
--- a/TestTable.xlsx
+++ b/TestTable.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phoenix/Desktop/OSU/ENGR 102/Code/HW3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F86CCA-90C6-7B43-BD5F-ED5E0116B208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A8EC0C-555F-124A-B65B-7039A346EEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44300" yWindow="1000" windowWidth="44800" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="0" windowWidth="43580" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Pass?
 (Does Expected = Actual?)</t>
@@ -32,20 +45,44 @@
     <t>(results are from the Python function)</t>
   </si>
   <si>
-    <t>est Case</t>
+    <t>Test Case</t>
   </si>
   <si>
-    <t>Actual</t>
+    <t>mu (mean)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Expected</t>
+    <t>sigma (standard deviation)</t>
+  </si>
+  <si>
+    <t>Column A</t>
+  </si>
+  <si>
+    <t>Column B</t>
+  </si>
+  <si>
+    <t>Column C</t>
+  </si>
+  <si>
+    <t>Test x</t>
+  </si>
+  <si>
+    <t>z-score (expected)</t>
+  </si>
+  <si>
+    <t>z-score (actual)</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -64,6 +101,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -111,6 +155,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -331,34 +385,40 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="31.33203125" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -378,95 +438,282 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <f>AVERAGE(A20:A22)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="8">
+        <f>_xlfn.STDEV.P(A20:A22)</f>
+        <v>0.81649658092772603</v>
+      </c>
+      <c r="E2" s="8">
+        <f>(B2-C2)/D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <f>AVERAGE(B20:B29)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <f>_xlfn.STDEV.P(B20:B29)</f>
+        <v>5.7445626465380286</v>
+      </c>
+      <c r="E3" s="8">
+        <f>(B3-C3)/D3</f>
+        <v>0.69631062382279141</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.69631062382279096</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <f>AVERAGE(C20:C32)</f>
+        <v>15.461538461538462</v>
+      </c>
+      <c r="D4" s="8">
+        <f>_xlfn.STDEV.P(C20:C32)</f>
+        <v>42.291325505566171</v>
+      </c>
+      <c r="E4" s="8">
+        <f>(B4-C4)/D4</f>
+        <v>-0.29465944404836253</v>
+      </c>
+      <c r="F4" s="8">
+        <v>-0.29465944404836197</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="4" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7">
+        <v>-3</v>
+      </c>
+      <c r="C21" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="7">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7">
+        <v>-5</v>
+      </c>
+      <c r="C22" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="7">
+        <v>-7</v>
+      </c>
+      <c r="C23" s="7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="7">
+        <v>-9</v>
+      </c>
+      <c r="C24" s="7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="7">
+        <v>9</v>
+      </c>
+      <c r="C25" s="7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="7">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="7">
+        <v>5</v>
+      </c>
+      <c r="C27" s="7">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="7">
+        <v>3</v>
+      </c>
+      <c r="C28" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C30" s="7">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C31" s="7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C32" s="7">
+        <v>42</v>
+      </c>
+    </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>